<commit_message>
added: empty row cells management
</commit_message>
<xml_diff>
--- a/samples/test.xlsx
+++ b/samples/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\dev\github\nano-csv\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1214C0E3-BB62-477B-A58E-A76D1E197A71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{182E379B-47CA-4261-8F70-FB45A04CF657}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{F5EE23E2-C2DE-4E29-85E7-DC5510388CE1}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
   <si>
     <t>cat</t>
   </si>
@@ -67,10 +67,16 @@
     <t>mammal</t>
   </si>
   <si>
-    <t>birds</t>
-  </si>
-  <si>
     <t>bat</t>
+  </si>
+  <si>
+    <t>bird</t>
+  </si>
+  <si>
+    <t>height</t>
+  </si>
+  <si>
+    <t>empty</t>
   </si>
 </sst>
 </file>
@@ -422,15 +428,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8194C91-71F3-475D-9220-4C91F9473F8C}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -440,8 +446,14 @@
       <c r="C1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -451,8 +463,11 @@
       <c r="C2">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -462,8 +477,11 @@
       <c r="C3">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -473,8 +491,11 @@
       <c r="C4">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -484,19 +505,25 @@
       <c r="C5">
         <v>30</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C6">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -506,15 +533,21 @@
       <c r="C7">
         <v>300</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
       </c>
       <c r="C8">
+        <v>0.1</v>
+      </c>
+      <c r="E8">
         <v>0.1</v>
       </c>
     </row>

</xml_diff>